<commit_message>
Tentativa com número de blocos maior
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -470,13 +470,13 @@
         <v>0.847531847133758</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.565246249834063</v>
+        <v>0.5652462498340635</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.757563694267516</v>
+        <v>0.7575636942675159</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.92942612942613</v>
+        <v>0.9294261294261295</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="4" s="4" spans="1:5">
@@ -484,13 +484,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.86897488119484</v>
+        <v>0.8689748811948405</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0.6614987080103359</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.7528852681602169</v>
+        <v>0.7528852681602173</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>0.9460439326082321</v>

</xml_diff>